<commit_message>
added more summary data
</commit_message>
<xml_diff>
--- a/data/20191114-193231/nunnerbuskens/numeric/summary.xlsx
+++ b/data/20191114-193231/nunnerbuskens/numeric/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hendrik\git\NIDM\simulation\data\20191114-193231\nunnerbuskens\numeric\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1DF241-6FEC-4E17-87CB-3A60C000ED7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69538D91-1DE5-44A7-9FBF-1E9CFC41C8D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="915" windowWidth="31635" windowHeight="19290" xr2:uid="{793F7540-6804-48A1-B221-E7610EE44690}"/>
+    <workbookView xWindow="28230" yWindow="9165" windowWidth="31635" windowHeight="19290" xr2:uid="{793F7540-6804-48A1-B221-E7610EE44690}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>alpha</t>
-  </si>
-  <si>
-    <t>N = 20</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>n</t>
   </si>
@@ -46,13 +40,64 @@
   </si>
   <si>
     <t>av. degree</t>
+  </si>
+  <si>
+    <t>clustering</t>
+  </si>
+  <si>
+    <t>av. path length</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>general settings</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>c1</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>triads</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>iota</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>alpha1</t>
+  </si>
+  <si>
+    <t>()</t>
+  </si>
+  <si>
+    <t>(0.05)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,10 +114,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,16 +148,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,163 +490,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14EC809-F148-4874-BA39-19508B58BFBC}">
-  <dimension ref="A2:J8"/>
+  <dimension ref="A3:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="10" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>0.5</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C5" s="4">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="4">
         <v>0.6</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E5" s="4">
         <v>0.65</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F5" s="4">
         <v>0.7</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G5" s="4">
         <v>0.75</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H5" s="4">
         <v>0.8</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I5" s="4">
         <v>0.85</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J5" s="4">
         <v>0.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-      <c r="I5">
-        <v>100</v>
-      </c>
-      <c r="J5">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="5">
+        <v>100</v>
+      </c>
+      <c r="C6" s="5">
+        <v>100</v>
+      </c>
+      <c r="D6" s="5">
+        <v>100</v>
+      </c>
+      <c r="E6" s="5">
+        <v>100</v>
+      </c>
+      <c r="F6" s="5">
+        <v>100</v>
+      </c>
+      <c r="G6" s="5">
+        <v>100</v>
+      </c>
+      <c r="H6" s="5">
+        <v>100</v>
+      </c>
+      <c r="I6" s="5">
+        <v>100</v>
+      </c>
+      <c r="J6" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5">
+        <v>0</v>
+      </c>
+      <c r="C7" s="5">
+        <v>10</v>
+      </c>
+      <c r="D7" s="5">
+        <v>52</v>
+      </c>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>60</v>
+      </c>
+      <c r="G7" s="5">
+        <v>36</v>
+      </c>
+      <c r="H7" s="5">
+        <v>14</v>
+      </c>
+      <c r="I7" s="5">
+        <v>29</v>
+      </c>
+      <c r="J7" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="6">
+        <v>7.62</v>
+      </c>
+      <c r="C9" s="6">
+        <v>7.23</v>
+      </c>
+      <c r="D9" s="7">
+        <v>7.02</v>
+      </c>
+      <c r="E9" s="7">
+        <v>7.08</v>
+      </c>
+      <c r="F9" s="7">
+        <v>6.61</v>
+      </c>
+      <c r="G9" s="7">
+        <v>6.54</v>
+      </c>
+      <c r="H9" s="7">
+        <v>6.58</v>
+      </c>
+      <c r="I9" s="7">
+        <v>6.42</v>
+      </c>
+      <c r="J9" s="7">
+        <v>5.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
+      <c r="B11" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.54</v>
+      </c>
+      <c r="D11" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="E11" s="6">
+        <v>0.65</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0.67</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.73</v>
+      </c>
+      <c r="I11" s="6">
+        <v>0.76</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6">
+        <v>1.64</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.71</v>
+      </c>
+      <c r="D13" s="6">
+        <v>1.83</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1.89</v>
+      </c>
+      <c r="F13" s="6">
+        <v>1.88</v>
+      </c>
+      <c r="G13" s="6">
+        <v>1.93</v>
+      </c>
+      <c r="H13" s="6">
+        <v>1.97</v>
+      </c>
+      <c r="I13" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="J13" s="6">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6">
-        <v>52</v>
-      </c>
-      <c r="E6">
-        <v>10</v>
-      </c>
-      <c r="F6">
-        <v>60</v>
-      </c>
-      <c r="G6">
-        <v>36</v>
-      </c>
-      <c r="H6">
+      <c r="F19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6">
-        <v>29</v>
-      </c>
-      <c r="J6">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>7.62</v>
-      </c>
-      <c r="C8">
-        <v>7.23</v>
-      </c>
-      <c r="D8" s="3">
-        <v>7.02</v>
-      </c>
-      <c r="E8" s="3">
-        <v>7.08</v>
-      </c>
-      <c r="F8" s="3">
-        <v>6.61</v>
-      </c>
-      <c r="G8" s="3">
-        <v>6.54</v>
-      </c>
-      <c r="H8" s="3">
-        <v>6.58</v>
-      </c>
-      <c r="I8" s="3">
-        <v>6.42</v>
-      </c>
-      <c r="J8" s="3">
-        <v>5.66</v>
-      </c>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="9">
+        <v>20</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="J20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>